<commit_message>
update file via upload
</commit_message>
<xml_diff>
--- a/Computer_User_Excel.xlsx
+++ b/Computer_User_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoftapc-my.sharepoint.com/personal/chosangho_microsoft_com/Documents/Desktop/yomihw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_F25DC773A252ABDACC1048DA699860E85BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5800E31-B294-4BF5-B092-0764CBA0B6EB}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC1048DA699860E85BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92883952-3F34-4DFA-9E06-53D82BE33506}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="59">
   <si>
     <t>Iris data set</t>
   </si>
@@ -137,6 +137,150 @@
     <t>Hint!
 Python in Excel uses the pandas library to create the DataFrame object in cell G2. Select the icon in the cell labeled DataFrame to see the output. Select the cell and expand the formula bar to see an example of how to create a DataFrame.
 Select cell G4 and expand the formula bar to see an example of the pandas describe function in a Python formula.</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>202.173.211.30</t>
+  </si>
+  <si>
+    <t>220.77.140.189</t>
+  </si>
+  <si>
+    <t>104.219.147.51</t>
+  </si>
+  <si>
+    <t>118.100.228.125</t>
+  </si>
+  <si>
+    <t>47.88.198.17</t>
+  </si>
+  <si>
+    <t>195.204.232.90</t>
+  </si>
+  <si>
+    <t>163.172.209.4</t>
+  </si>
+  <si>
+    <t>181.114.23.70</t>
+  </si>
+  <si>
+    <t>188.166.83.29</t>
+  </si>
+  <si>
+    <t>217.182.82.44</t>
+  </si>
+  <si>
+    <t>213.186.34.99</t>
+  </si>
+  <si>
+    <t>45.76.171.247</t>
+  </si>
+  <si>
+    <t>174.138.60.54</t>
+  </si>
+  <si>
+    <t>109.234.36.6</t>
+  </si>
+  <si>
+    <t>103.212.223.245</t>
+  </si>
+  <si>
+    <t>185.212.254.201</t>
+  </si>
+  <si>
+    <t>187.86.67.85</t>
+  </si>
+  <si>
+    <t>122.248.242.239</t>
+  </si>
+  <si>
+    <t>139.59.74.233</t>
+  </si>
+  <si>
+    <t>64.225.116.175</t>
+  </si>
+  <si>
+    <t>91.121.134.148</t>
+  </si>
+  <si>
+    <t>208.113.194.28</t>
+  </si>
+  <si>
+    <t>212.227.42.43</t>
+  </si>
+  <si>
+    <t>222.124.154.58</t>
+  </si>
+  <si>
+    <t>78.46.80.230</t>
+  </si>
+  <si>
+    <t>79.137.57.130</t>
+  </si>
+  <si>
+    <t>89.40.14.207</t>
+  </si>
+  <si>
+    <t>190.216.224.37</t>
+  </si>
+  <si>
+    <t>92.249.122.39</t>
+  </si>
+  <si>
+    <t>98.158.178.141</t>
+  </si>
+  <si>
+    <t>165.227.63.87</t>
+  </si>
+  <si>
+    <t>36.92.117.143</t>
+  </si>
+  <si>
+    <t>185.150.92.21</t>
+  </si>
+  <si>
+    <t>103.27.206.205</t>
+  </si>
+  <si>
+    <t>68.183.102.32</t>
+  </si>
+  <si>
+    <t>83.96.252.206</t>
+  </si>
+  <si>
+    <t>190.2.210.237</t>
+  </si>
+  <si>
+    <t>176.9.145.194</t>
+  </si>
+  <si>
+    <t>178.128.50.114</t>
+  </si>
+  <si>
+    <t>1.20.97.227</t>
+  </si>
+  <si>
+    <t>159.69.120.129</t>
+  </si>
+  <si>
+    <t>64.150.191.231</t>
+  </si>
+  <si>
+    <t>103.195.100.47</t>
+  </si>
+  <si>
+    <t>185.122.58.233</t>
+  </si>
+  <si>
+    <t>202.152.38.77</t>
+  </si>
+  <si>
+    <t>157.230.253.101</t>
   </si>
 </sst>
 </file>
@@ -268,20 +412,20 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -781,13 +925,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -795,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E660E7-D94C-49F0-89CB-EE0201047432}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1174,12 +1565,12 @@
       <c r="E14" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="10"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1197,10 +1588,10 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="11"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1218,10 +1609,10 @@
       <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="11"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -1239,10 +1630,10 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="11"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
@@ -1260,10 +1651,10 @@
       <c r="E18" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="11"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
@@ -1281,10 +1672,10 @@
       <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="11"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -1302,10 +1693,10 @@
       <c r="E20" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="11"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21">
@@ -1323,9 +1714,9 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -3556,13 +3947,13 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>